<commit_message>
station delft in tabel
</commit_message>
<xml_diff>
--- a/tp3.xlsx
+++ b/tp3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6729ADD7-391E-4508-9719-81E34E2C46DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCA43AF-8340-4115-A90B-EB36E6435592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{37FD1C8F-5E12-4B60-99E0-C984E3A475B4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Bezienswaardigheden</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>Actief</t>
+  </si>
+  <si>
+    <t>Station Delft, 2611 AC Delft</t>
+  </si>
+  <si>
+    <t>Station Delft</t>
+  </si>
+  <si>
+    <t>begin_eindpunt</t>
   </si>
 </sst>
 </file>
@@ -641,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB7E1BF-E5C9-4D55-8B2F-C00324E2772D}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="89" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="89" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -650,7 +659,7 @@
     <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="72.08984375" customWidth="1"/>
     <col min="3" max="3" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
     <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.81640625" bestFit="1" customWidth="1"/>
@@ -1308,6 +1317,20 @@
       </c>
       <c r="D25" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>